<commit_message>
Updated RTM and Delivery History Signed-off-by: moamen-ahmed-93 <moamen.ahmed.9930@gmail.com>
</commit_message>
<xml_diff>
--- a/Software specification/RTM.xlsx
+++ b/Software specification/RTM.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22325"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22430"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Moamen\Desktop\SWE\Software specification\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C474CBDC-D5A4-4FAA-A676-FFE1E98FB592}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3EE5007-6290-4CE4-BE54-214D83FE89BA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_Toc30697436" localSheetId="0">Sheet1!$I$5</definedName>
+    <definedName name="_Toc30697436" localSheetId="0">Sheet1!$I$11</definedName>
   </definedNames>
   <calcPr calcId="0"/>
   <extLst>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="53">
   <si>
     <t>Requirment ID</t>
   </si>
@@ -60,42 +60,24 @@
     <t>Req_ PO1_DGC_CRS_01_V1.0</t>
   </si>
   <si>
-    <t>Req_PO1_DGC_CYRS_001_v1.0</t>
-  </si>
-  <si>
     <t>v1.0</t>
   </si>
   <si>
-    <t>Draft</t>
-  </si>
-  <si>
-    <t>Req_PO1_DGC_CYRS_002_v1.0</t>
-  </si>
-  <si>
     <t>Req_PO1_DGC_SRS_001_v1.0</t>
   </si>
   <si>
     <t>Req_ PO1_DGC_CRS_02_V1.0</t>
   </si>
   <si>
-    <t>The user should enter the numbers and select the operations need</t>
-  </si>
-  <si>
     <t>Req_PO1_DGC_CYRS_003_v1.0</t>
   </si>
   <si>
     <t>Req_PO1_DGC_SRS_002_v1.0</t>
   </si>
   <si>
-    <t>Req_PO1_DGC_CYRS_004_v1.0</t>
-  </si>
-  <si>
     <t>Req_PO1_DGC_SRS_003_v1.0</t>
   </si>
   <si>
-    <t>Req_PO1_DGC_CYRS_005_v1.0</t>
-  </si>
-  <si>
     <t>Req_PO1_DGC_SRS_004_v1.0</t>
   </si>
   <si>
@@ -105,12 +87,6 @@
     <t>Req_ PO1_DGC_CRS_03_V1.0</t>
   </si>
   <si>
-    <t>Both the operations and result shall be appeared on a display.</t>
-  </si>
-  <si>
-    <t>Req_PO1_DGC_CYRS_006_v1.1</t>
-  </si>
-  <si>
     <t>v1.1</t>
   </si>
   <si>
@@ -123,13 +99,7 @@
     <t>Req_PO1_DGC_SRS_008_v1.0</t>
   </si>
   <si>
-    <t>Req_PO1_DGC_SRS_009_v1.0</t>
-  </si>
-  <si>
     <t>When the user press any key , it must be followed by a tune</t>
-  </si>
-  <si>
-    <t>Req_PO1_DGC_CYRS_007_v1.0</t>
   </si>
   <si>
     <t>Req_PO1_DGC_SRS_010_v1.0</t>
@@ -152,6 +122,72 @@
   </si>
   <si>
     <t>HWC_DGC_HSI_003_v1.1</t>
+  </si>
+  <si>
+    <t>Req_PO1_DGC_CYRS_001_v1.1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Req_PO1_DGC_CYRS_002_v1.2 </t>
+  </si>
+  <si>
+    <t>Req_PO1_DGC_CYRS_004_v1.1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Req_PO1_DGC_CYRS_005_v1.0 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Req_PO1_DGC_CYRS_006_v1.1 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Req_PO1_DGC_CYRS_007_v1.1 </t>
+  </si>
+  <si>
+    <t>v1.2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Req_PO1_DGC_CYRS_008_v1.0 </t>
+  </si>
+  <si>
+    <t>The user should enter the numbers and select the operation</t>
+  </si>
+  <si>
+    <t>Pressing the equal button displays both the operations and result.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Req_PO1_DGC_CYRS_009_v1.0 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Req_PO1_DGC_CYRS_010_v1.0 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Req_PO1_DGC_CYRS_011_v1.0 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Req_PO1_DGC_CYRS_012_v1.0 </t>
+  </si>
+  <si>
+    <t>Req_PO1_DGC_SRS_0010_v1.0</t>
+  </si>
+  <si>
+    <t>Req_PO1_DGC_SRS_0011_v1.0</t>
+  </si>
+  <si>
+    <t>Req_PO1_DGC_SRS_0012_v1.0</t>
+  </si>
+  <si>
+    <t>Req_PO1_DGC_SRS_0013_v1.0</t>
+  </si>
+  <si>
+    <t>Req_PO1_DGC_SRS_0014_v1.0</t>
+  </si>
+  <si>
+    <t>Req_PO1_DGC_SRS_0015_v1.0</t>
+  </si>
+  <si>
+    <t>Req_PO1_DGC_SRS_0016_v1.0</t>
+  </si>
+  <si>
+    <t>Req_PO1_DGC_SRS_0017_v1.0</t>
   </si>
 </sst>
 </file>
@@ -181,17 +217,18 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
@@ -210,7 +247,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="8">
+  <borders count="14">
     <border>
       <left/>
       <right/>
@@ -299,6 +336,78 @@
       </right>
       <top style="thin">
         <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
       </top>
       <bottom style="thin">
         <color indexed="64"/>
@@ -309,15 +418,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="41">
+  <cellXfs count="67">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -331,48 +437,27 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -399,30 +484,126 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -640,10 +821,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L999"/>
+  <dimension ref="A1:L1005"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B27" sqref="B27"/>
+      <selection activeCell="F29" sqref="F29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -651,13 +832,13 @@
     <col min="1" max="1" width="29.140625" customWidth="1"/>
     <col min="2" max="2" width="61.7109375" customWidth="1"/>
     <col min="3" max="3" width="43" customWidth="1"/>
-    <col min="4" max="4" width="8.7109375" customWidth="1"/>
+    <col min="4" max="4" width="8.7109375" hidden="1" customWidth="1"/>
     <col min="5" max="5" width="13.42578125" customWidth="1"/>
-    <col min="6" max="6" width="27.28515625" customWidth="1"/>
-    <col min="7" max="7" width="8.7109375" customWidth="1"/>
+    <col min="6" max="6" width="29.5703125" customWidth="1"/>
+    <col min="7" max="7" width="8.7109375" hidden="1" customWidth="1"/>
     <col min="8" max="8" width="11.140625" customWidth="1"/>
     <col min="9" max="9" width="23.42578125" customWidth="1"/>
-    <col min="10" max="10" width="8.7109375" customWidth="1"/>
+    <col min="10" max="10" width="8.7109375" hidden="1" customWidth="1"/>
     <col min="11" max="11" width="10.5703125" customWidth="1"/>
     <col min="12" max="12" width="8.7109375" customWidth="1"/>
   </cols>
@@ -698,420 +879,514 @@
       </c>
     </row>
     <row r="2" spans="1:12" ht="14.25" customHeight="1">
-      <c r="A2" s="31" t="s">
+      <c r="A2" s="27" t="s">
         <v>9</v>
       </c>
-      <c r="B2" s="36" t="s">
+      <c r="B2" s="48" t="s">
+        <v>25</v>
+      </c>
+      <c r="C2" s="49" t="s">
+        <v>31</v>
+      </c>
+      <c r="D2" s="24" t="s">
+        <v>19</v>
+      </c>
+      <c r="E2" s="24"/>
+      <c r="F2" s="3"/>
+      <c r="G2" s="4"/>
+      <c r="H2" s="4"/>
+      <c r="I2" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="J2" s="4"/>
+      <c r="K2" s="24" t="s">
+        <v>27</v>
+      </c>
+      <c r="L2" s="6"/>
+    </row>
+    <row r="3" spans="1:12" ht="14.25" customHeight="1">
+      <c r="A3" s="30"/>
+      <c r="B3" s="45"/>
+      <c r="C3" s="50" t="s">
+        <v>32</v>
+      </c>
+      <c r="D3" s="32" t="s">
+        <v>37</v>
+      </c>
+      <c r="E3" s="12"/>
+      <c r="F3" s="56" t="s">
+        <v>11</v>
+      </c>
+      <c r="G3" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="H3" s="37" t="s">
+        <v>27</v>
+      </c>
+      <c r="I3" s="31" t="s">
+        <v>28</v>
+      </c>
+      <c r="J3" s="9"/>
+      <c r="K3" s="37" t="s">
+        <v>27</v>
+      </c>
+      <c r="L3" s="6"/>
+    </row>
+    <row r="4" spans="1:12" ht="14.25" customHeight="1">
+      <c r="A4" s="30"/>
+      <c r="B4" s="45"/>
+      <c r="C4" s="50"/>
+      <c r="D4" s="43"/>
+      <c r="E4" s="12"/>
+      <c r="F4" s="56" t="s">
+        <v>14</v>
+      </c>
+      <c r="G4" s="38"/>
+      <c r="H4" s="37" t="s">
+        <v>27</v>
+      </c>
+      <c r="I4" s="31"/>
+      <c r="J4" s="12"/>
+      <c r="K4" s="37"/>
+      <c r="L4" s="6"/>
+    </row>
+    <row r="5" spans="1:12" ht="14.25" customHeight="1">
+      <c r="A5" s="30"/>
+      <c r="B5" s="45"/>
+      <c r="C5" s="44" t="s">
+        <v>41</v>
+      </c>
+      <c r="D5" s="43"/>
+      <c r="E5" s="12"/>
+      <c r="F5" s="56" t="s">
+        <v>47</v>
+      </c>
+      <c r="G5" s="38"/>
+      <c r="H5" s="37" t="s">
+        <v>27</v>
+      </c>
+      <c r="I5" s="31"/>
+      <c r="J5" s="38"/>
+      <c r="K5" s="65"/>
+      <c r="L5" s="6"/>
+    </row>
+    <row r="6" spans="1:12" ht="14.25" customHeight="1">
+      <c r="A6" s="30"/>
+      <c r="B6" s="45"/>
+      <c r="C6" s="51" t="s">
+        <v>42</v>
+      </c>
+      <c r="D6" s="43"/>
+      <c r="E6" s="12"/>
+      <c r="F6" s="56" t="s">
+        <v>48</v>
+      </c>
+      <c r="G6" s="38"/>
+      <c r="H6" s="37" t="s">
+        <v>27</v>
+      </c>
+      <c r="I6" s="31"/>
+      <c r="J6" s="38"/>
+      <c r="K6" s="65"/>
+      <c r="L6" s="6"/>
+    </row>
+    <row r="7" spans="1:12" ht="14.25" customHeight="1">
+      <c r="A7" s="30"/>
+      <c r="B7" s="45"/>
+      <c r="C7" s="51"/>
+      <c r="D7" s="43"/>
+      <c r="E7" s="12"/>
+      <c r="F7" s="56" t="s">
+        <v>49</v>
+      </c>
+      <c r="G7" s="38"/>
+      <c r="H7" s="37" t="s">
+        <v>27</v>
+      </c>
+      <c r="I7" s="31"/>
+      <c r="J7" s="38"/>
+      <c r="K7" s="65"/>
+      <c r="L7" s="6"/>
+    </row>
+    <row r="8" spans="1:12" ht="14.25" customHeight="1">
+      <c r="A8" s="30"/>
+      <c r="B8" s="45"/>
+      <c r="C8" s="51" t="s">
+        <v>43</v>
+      </c>
+      <c r="D8" s="43"/>
+      <c r="E8" s="12"/>
+      <c r="F8" s="56" t="s">
+        <v>50</v>
+      </c>
+      <c r="G8" s="38"/>
+      <c r="H8" s="37" t="s">
+        <v>27</v>
+      </c>
+      <c r="I8" s="31"/>
+      <c r="J8" s="38"/>
+      <c r="K8" s="65"/>
+      <c r="L8" s="6"/>
+    </row>
+    <row r="9" spans="1:12" ht="14.25" customHeight="1">
+      <c r="A9" s="40"/>
+      <c r="B9" s="42"/>
+      <c r="C9" s="52"/>
+      <c r="D9" s="43"/>
+      <c r="E9" s="12"/>
+      <c r="F9" s="56" t="s">
+        <v>51</v>
+      </c>
+      <c r="G9" s="38"/>
+      <c r="H9" s="63" t="s">
+        <v>27</v>
+      </c>
+      <c r="I9" s="31"/>
+      <c r="J9" s="38"/>
+      <c r="K9" s="66"/>
+      <c r="L9" s="6"/>
+    </row>
+    <row r="10" spans="1:12" ht="14.25" customHeight="1">
+      <c r="A10" s="27" t="s">
+        <v>12</v>
+      </c>
+      <c r="B10" s="34" t="s">
+        <v>39</v>
+      </c>
+      <c r="C10" s="53" t="s">
+        <v>13</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E10" s="2"/>
+      <c r="F10" s="57" t="s">
+        <v>15</v>
+      </c>
+      <c r="G10" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="H10" s="37" t="s">
+        <v>27</v>
+      </c>
+      <c r="I10" s="25" t="s">
+        <v>28</v>
+      </c>
+      <c r="J10" s="4"/>
+      <c r="K10" s="37" t="s">
+        <v>27</v>
+      </c>
+      <c r="L10" s="6"/>
+    </row>
+    <row r="11" spans="1:12" ht="14.25" customHeight="1">
+      <c r="A11" s="30"/>
+      <c r="B11" s="33"/>
+      <c r="C11" s="50" t="s">
+        <v>33</v>
+      </c>
+      <c r="D11" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="E11" s="11"/>
+      <c r="F11" s="58" t="s">
+        <v>16</v>
+      </c>
+      <c r="G11" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="H11" s="37" t="s">
+        <v>27</v>
+      </c>
+      <c r="I11" s="12"/>
+      <c r="J11" s="12"/>
+      <c r="K11" s="12"/>
+      <c r="L11" s="6"/>
+    </row>
+    <row r="12" spans="1:12" ht="14.25" customHeight="1">
+      <c r="A12" s="30"/>
+      <c r="B12" s="33"/>
+      <c r="C12" s="50"/>
+      <c r="D12" s="12"/>
+      <c r="E12" s="12"/>
+      <c r="F12" s="58" t="s">
+        <v>17</v>
+      </c>
+      <c r="G12" s="12"/>
+      <c r="H12" s="37" t="s">
+        <v>27</v>
+      </c>
+      <c r="I12" s="13"/>
+      <c r="J12" s="12"/>
+      <c r="K12" s="12"/>
+      <c r="L12" s="6"/>
+    </row>
+    <row r="13" spans="1:12" ht="14.25" customHeight="1">
+      <c r="A13" s="30"/>
+      <c r="B13" s="33"/>
+      <c r="C13" s="61" t="s">
+        <v>34</v>
+      </c>
+      <c r="D13" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="E13" s="12"/>
+      <c r="F13" s="58" t="s">
+        <v>20</v>
+      </c>
+      <c r="G13" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="H13" s="37" t="s">
+        <v>27</v>
+      </c>
+      <c r="I13" s="13"/>
+      <c r="J13" s="12"/>
+      <c r="K13" s="12"/>
+      <c r="L13" s="6"/>
+    </row>
+    <row r="14" spans="1:12" ht="15" customHeight="1">
+      <c r="A14" s="30"/>
+      <c r="B14" s="33"/>
+      <c r="C14" s="61"/>
+      <c r="D14" s="30" t="s">
+        <v>10</v>
+      </c>
+      <c r="E14" s="46"/>
+      <c r="F14" s="58" t="s">
+        <v>21</v>
+      </c>
+      <c r="G14" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="H14" s="37" t="s">
+        <v>27</v>
+      </c>
+      <c r="I14" s="14"/>
+      <c r="J14" s="12"/>
+      <c r="K14" s="14"/>
+      <c r="L14" s="6"/>
+    </row>
+    <row r="15" spans="1:12" ht="15" customHeight="1">
+      <c r="A15" s="30"/>
+      <c r="B15" s="33"/>
+      <c r="C15" s="33" t="s">
+        <v>38</v>
+      </c>
+      <c r="D15" s="29"/>
+      <c r="E15" s="46"/>
+      <c r="F15" s="58" t="s">
+        <v>45</v>
+      </c>
+      <c r="G15" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="H15" s="37" t="s">
+        <v>27</v>
+      </c>
+      <c r="I15" s="14"/>
+      <c r="J15" s="9"/>
+      <c r="K15" s="14"/>
+      <c r="L15" s="6"/>
+    </row>
+    <row r="16" spans="1:12" ht="15" customHeight="1">
+      <c r="A16" s="40"/>
+      <c r="B16" s="62"/>
+      <c r="C16" s="62"/>
+      <c r="D16" s="23"/>
+      <c r="E16" s="47"/>
+      <c r="F16" s="59" t="s">
+        <v>46</v>
+      </c>
+      <c r="G16" s="12"/>
+      <c r="H16" s="63" t="s">
+        <v>27</v>
+      </c>
+      <c r="I16" s="8"/>
+      <c r="J16" s="12"/>
+      <c r="K16" s="8"/>
+      <c r="L16" s="6"/>
+    </row>
+    <row r="17" spans="1:12" ht="14.25" customHeight="1">
+      <c r="A17" s="27" t="s">
+        <v>18</v>
+      </c>
+      <c r="B17" s="34" t="s">
+        <v>40</v>
+      </c>
+      <c r="C17" s="35" t="s">
         <v>35</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="D17" s="27" t="s">
+        <v>19</v>
+      </c>
+      <c r="E17" s="39"/>
+      <c r="F17" s="60" t="s">
+        <v>22</v>
+      </c>
+      <c r="G17" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="D2" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="E2" s="37" t="s">
-        <v>37</v>
-      </c>
-      <c r="F2" s="4"/>
-      <c r="G2" s="5"/>
-      <c r="H2" s="5"/>
-      <c r="I2" s="6" t="s">
+      <c r="H17" s="37" t="s">
+        <v>27</v>
+      </c>
+      <c r="I17" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="J17" s="4"/>
+      <c r="K17" s="24" t="s">
+        <v>27</v>
+      </c>
+      <c r="L17" s="6"/>
+    </row>
+    <row r="18" spans="1:12" ht="14.25" customHeight="1">
+      <c r="A18" s="30"/>
+      <c r="B18" s="33"/>
+      <c r="C18" s="55" t="s">
+        <v>44</v>
+      </c>
+      <c r="D18" s="28"/>
+      <c r="E18" s="36"/>
+      <c r="F18" s="58" t="s">
+        <v>52</v>
+      </c>
+      <c r="G18" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="H18" s="37" t="s">
+        <v>27</v>
+      </c>
+      <c r="I18" s="14"/>
+      <c r="J18" s="12"/>
+      <c r="K18" s="14"/>
+      <c r="L18" s="6"/>
+    </row>
+    <row r="19" spans="1:12" ht="14.25" customHeight="1">
+      <c r="A19" s="15" t="s">
+        <v>18</v>
+      </c>
+      <c r="B19" s="15" t="s">
+        <v>23</v>
+      </c>
+      <c r="C19" s="54" t="s">
         <v>36</v>
       </c>
-      <c r="J2" s="5"/>
-      <c r="K2" s="37" t="s">
-        <v>37</v>
-      </c>
-      <c r="L2" s="7"/>
-    </row>
-    <row r="3" spans="1:12" ht="14.25" customHeight="1">
-      <c r="A3" s="33"/>
-      <c r="B3" s="33"/>
-      <c r="C3" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="D3" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="E3" s="9" t="s">
-        <v>37</v>
-      </c>
-      <c r="F3" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="G3" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="H3" s="9" t="s">
-        <v>12</v>
-      </c>
-      <c r="I3" s="38" t="s">
-        <v>38</v>
-      </c>
-      <c r="J3" s="11"/>
-      <c r="K3" s="37" t="s">
-        <v>37</v>
-      </c>
-      <c r="L3" s="7"/>
-    </row>
-    <row r="4" spans="1:12" ht="14.25" customHeight="1">
-      <c r="A4" s="31" t="s">
-        <v>15</v>
-      </c>
-      <c r="B4" s="31" t="s">
-        <v>16</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="D4" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="E4" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="F4" s="12" t="s">
-        <v>14</v>
-      </c>
-      <c r="G4" s="13" t="s">
-        <v>11</v>
-      </c>
-      <c r="H4" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="I4" s="39" t="s">
-        <v>38</v>
-      </c>
-      <c r="J4" s="5"/>
-      <c r="K4" s="37" t="s">
-        <v>37</v>
-      </c>
-      <c r="L4" s="7"/>
-    </row>
-    <row r="5" spans="1:12" ht="14.25" customHeight="1">
-      <c r="A5" s="32"/>
-      <c r="B5" s="32"/>
-      <c r="C5" s="14" t="s">
-        <v>17</v>
-      </c>
-      <c r="D5" s="15" t="s">
-        <v>11</v>
-      </c>
-      <c r="E5" s="15" t="s">
-        <v>37</v>
-      </c>
-      <c r="F5" s="15" t="s">
-        <v>18</v>
-      </c>
-      <c r="G5" s="15" t="s">
-        <v>11</v>
-      </c>
-      <c r="H5" s="16" t="s">
-        <v>12</v>
-      </c>
-      <c r="I5" s="17"/>
-      <c r="J5" s="17"/>
-      <c r="K5" s="17"/>
-      <c r="L5" s="7"/>
-    </row>
-    <row r="6" spans="1:12" ht="14.25" customHeight="1">
-      <c r="A6" s="32"/>
-      <c r="B6" s="32"/>
-      <c r="C6" s="18" t="s">
-        <v>19</v>
-      </c>
-      <c r="D6" s="15" t="s">
-        <v>11</v>
-      </c>
-      <c r="E6" s="17" t="s">
-        <v>37</v>
-      </c>
-      <c r="F6" s="15" t="s">
-        <v>20</v>
-      </c>
-      <c r="G6" s="15" t="s">
-        <v>11</v>
-      </c>
-      <c r="H6" s="16" t="s">
-        <v>12</v>
-      </c>
-      <c r="I6" s="19"/>
-      <c r="J6" s="17"/>
-      <c r="K6" s="17"/>
-      <c r="L6" s="7"/>
-    </row>
-    <row r="7" spans="1:12" ht="15" customHeight="1">
-      <c r="A7" s="32"/>
-      <c r="B7" s="32"/>
-      <c r="C7" s="35" t="s">
-        <v>21</v>
-      </c>
-      <c r="D7" s="35" t="s">
-        <v>11</v>
-      </c>
-      <c r="E7" s="35" t="s">
-        <v>37</v>
-      </c>
-      <c r="F7" s="15" t="s">
-        <v>22</v>
-      </c>
-      <c r="G7" s="15" t="s">
-        <v>11</v>
-      </c>
-      <c r="H7" s="16" t="s">
-        <v>12</v>
-      </c>
-      <c r="I7" s="20"/>
-      <c r="J7" s="17"/>
-      <c r="K7" s="20"/>
-      <c r="L7" s="7"/>
-    </row>
-    <row r="8" spans="1:12" ht="15" customHeight="1">
-      <c r="A8" s="33"/>
-      <c r="B8" s="33"/>
-      <c r="C8" s="33"/>
-      <c r="D8" s="33"/>
-      <c r="E8" s="33"/>
-      <c r="F8" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="G8" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="H8" s="21" t="s">
-        <v>12</v>
-      </c>
-      <c r="I8" s="10"/>
-      <c r="J8" s="11"/>
-      <c r="K8" s="10"/>
-      <c r="L8" s="7"/>
-    </row>
-    <row r="9" spans="1:12" ht="14.25" customHeight="1">
-      <c r="A9" s="31" t="s">
+      <c r="D19" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="E19" s="17"/>
+      <c r="F19" s="15" t="s">
         <v>24</v>
       </c>
-      <c r="B9" s="31" t="s">
-        <v>25</v>
-      </c>
-      <c r="C9" s="34" t="s">
-        <v>26</v>
-      </c>
-      <c r="D9" s="31" t="s">
+      <c r="G19" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="H19" s="64" t="s">
         <v>27</v>
       </c>
-      <c r="E9" s="31" t="s">
-        <v>37</v>
-      </c>
-      <c r="F9" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="G9" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="H9" s="22" t="s">
-        <v>12</v>
-      </c>
-      <c r="I9" s="6" t="s">
-        <v>40</v>
-      </c>
-      <c r="J9" s="5"/>
-      <c r="K9" s="37" t="s">
-        <v>37</v>
-      </c>
-      <c r="L9" s="7"/>
-    </row>
-    <row r="10" spans="1:12" ht="14.25" customHeight="1">
-      <c r="A10" s="32"/>
-      <c r="B10" s="32"/>
-      <c r="C10" s="32"/>
-      <c r="D10" s="32"/>
-      <c r="E10" s="32"/>
-      <c r="F10" s="15" t="s">
+      <c r="I19" s="17" t="s">
         <v>29</v>
       </c>
-      <c r="G10" s="15" t="s">
-        <v>11</v>
-      </c>
-      <c r="H10" s="16" t="s">
-        <v>12</v>
-      </c>
-      <c r="I10" s="20"/>
-      <c r="J10" s="17"/>
-      <c r="K10" s="20"/>
-      <c r="L10" s="7"/>
-    </row>
-    <row r="11" spans="1:12" ht="14.25" customHeight="1">
-      <c r="A11" s="32"/>
-      <c r="B11" s="32"/>
-      <c r="C11" s="32"/>
-      <c r="D11" s="32"/>
-      <c r="E11" s="32"/>
-      <c r="F11" s="15" t="s">
-        <v>30</v>
-      </c>
-      <c r="G11" s="15" t="s">
-        <v>11</v>
-      </c>
-      <c r="H11" s="16" t="s">
-        <v>12</v>
-      </c>
-      <c r="I11" s="20"/>
-      <c r="J11" s="17"/>
-      <c r="K11" s="20"/>
-      <c r="L11" s="7"/>
-    </row>
-    <row r="12" spans="1:12" ht="14.25" customHeight="1">
-      <c r="A12" s="33"/>
-      <c r="B12" s="33"/>
-      <c r="C12" s="33"/>
-      <c r="D12" s="33"/>
-      <c r="E12" s="33"/>
-      <c r="F12" s="9" t="s">
-        <v>31</v>
-      </c>
-      <c r="G12" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="H12" s="21" t="s">
-        <v>12</v>
-      </c>
-      <c r="I12" s="10"/>
-      <c r="J12" s="11"/>
-      <c r="K12" s="10"/>
-      <c r="L12" s="7"/>
-    </row>
-    <row r="13" spans="1:12" ht="14.25" customHeight="1">
-      <c r="A13" s="23" t="s">
-        <v>24</v>
-      </c>
-      <c r="B13" s="23" t="s">
-        <v>32</v>
-      </c>
-      <c r="C13" s="24" t="s">
-        <v>33</v>
-      </c>
-      <c r="D13" s="24" t="s">
-        <v>11</v>
-      </c>
-      <c r="E13" s="25"/>
-      <c r="F13" s="24" t="s">
-        <v>34</v>
-      </c>
-      <c r="G13" s="24" t="s">
-        <v>11</v>
-      </c>
-      <c r="H13" s="24" t="s">
-        <v>12</v>
-      </c>
-      <c r="I13" s="25" t="s">
-        <v>39</v>
-      </c>
-      <c r="J13" s="25"/>
-      <c r="K13" s="40" t="s">
-        <v>37</v>
-      </c>
-      <c r="L13" s="7"/>
-    </row>
-    <row r="14" spans="1:12" ht="14.25" customHeight="1">
-      <c r="L14" s="7"/>
-    </row>
-    <row r="15" spans="1:12" ht="14.25" customHeight="1">
-      <c r="A15" s="26"/>
-      <c r="B15" s="26"/>
-      <c r="C15" s="26"/>
-      <c r="D15" s="26"/>
-      <c r="E15" s="26"/>
-      <c r="F15" s="26"/>
-      <c r="G15" s="26"/>
-      <c r="I15" s="26"/>
-      <c r="J15" s="26"/>
-      <c r="K15" s="26"/>
-      <c r="L15" s="7"/>
-    </row>
-    <row r="16" spans="1:12" ht="14.25" customHeight="1">
-      <c r="A16" s="26"/>
-      <c r="B16" s="26"/>
-      <c r="C16" s="26"/>
-      <c r="D16" s="27"/>
-      <c r="E16" s="28"/>
-      <c r="F16" s="26"/>
-      <c r="G16" s="28"/>
-      <c r="H16" s="29"/>
-      <c r="I16" s="26"/>
-      <c r="J16" s="26"/>
-      <c r="K16" s="26"/>
-      <c r="L16" s="7"/>
-    </row>
-    <row r="17" spans="1:12" ht="14.25" customHeight="1">
-      <c r="C17" s="27"/>
-      <c r="D17" s="27"/>
-      <c r="E17" s="28"/>
-      <c r="F17" s="28"/>
-      <c r="G17" s="28"/>
-      <c r="H17" s="28"/>
-      <c r="I17" s="28"/>
-      <c r="J17" s="28"/>
-      <c r="K17" s="28"/>
-      <c r="L17" s="7"/>
-    </row>
-    <row r="18" spans="1:12" ht="14.25" customHeight="1"/>
-    <row r="19" spans="1:12" ht="14.25" customHeight="1"/>
-    <row r="20" spans="1:12" ht="14.25" customHeight="1"/>
-    <row r="21" spans="1:12" ht="14.25" customHeight="1"/>
-    <row r="22" spans="1:12" ht="14.25" customHeight="1"/>
-    <row r="23" spans="1:12" ht="14.25" customHeight="1"/>
+      <c r="J19" s="17"/>
+      <c r="K19" s="26" t="s">
+        <v>27</v>
+      </c>
+      <c r="L19" s="6"/>
+    </row>
+    <row r="20" spans="1:12" ht="14.25" customHeight="1">
+      <c r="L20" s="6"/>
+    </row>
+    <row r="21" spans="1:12" ht="14.25" customHeight="1">
+      <c r="A21" s="18"/>
+      <c r="B21" s="18"/>
+      <c r="C21" s="18"/>
+      <c r="D21" s="18"/>
+      <c r="E21" s="18"/>
+      <c r="F21" s="18"/>
+      <c r="G21" s="18"/>
+      <c r="I21" s="18"/>
+      <c r="J21" s="18"/>
+      <c r="K21" s="18"/>
+      <c r="L21" s="6"/>
+    </row>
+    <row r="22" spans="1:12" ht="14.25" customHeight="1">
+      <c r="A22" s="18"/>
+      <c r="B22" s="18"/>
+      <c r="C22" s="18"/>
+      <c r="D22" s="19"/>
+      <c r="E22" s="20"/>
+      <c r="F22" s="18"/>
+      <c r="G22" s="20"/>
+      <c r="H22" s="21"/>
+      <c r="I22" s="18"/>
+      <c r="J22" s="18"/>
+      <c r="K22" s="18"/>
+      <c r="L22" s="6"/>
+    </row>
+    <row r="23" spans="1:12" ht="14.25" customHeight="1">
+      <c r="C23" s="19"/>
+      <c r="D23" s="19"/>
+      <c r="E23" s="20"/>
+      <c r="F23" s="20"/>
+      <c r="G23" s="20"/>
+      <c r="H23" s="20"/>
+      <c r="I23" s="20"/>
+      <c r="J23" s="20"/>
+      <c r="K23" s="20"/>
+      <c r="L23" s="6"/>
+    </row>
     <row r="24" spans="1:12" ht="14.25" customHeight="1"/>
     <row r="25" spans="1:12" ht="14.25" customHeight="1">
-      <c r="A25" s="26"/>
-      <c r="E25" s="26"/>
-      <c r="I25" s="26"/>
-      <c r="J25" s="26"/>
-      <c r="K25" s="26"/>
-    </row>
-    <row r="26" spans="1:12" ht="14.25" customHeight="1">
-      <c r="A26" s="26"/>
-      <c r="B26" s="26"/>
-      <c r="C26" s="30"/>
-      <c r="D26" s="26"/>
-      <c r="E26" s="26"/>
-      <c r="F26" s="26"/>
-      <c r="G26" s="26"/>
-      <c r="H26" s="26"/>
-      <c r="I26" s="26"/>
-      <c r="J26" s="26"/>
-      <c r="K26" s="26"/>
-    </row>
-    <row r="27" spans="1:12" ht="14.25" customHeight="1">
-      <c r="C27" s="30"/>
-    </row>
-    <row r="28" spans="1:12" ht="14.25" customHeight="1">
-      <c r="C28" s="30"/>
-    </row>
-    <row r="29" spans="1:12" ht="14.25" customHeight="1">
-      <c r="C29" s="30"/>
-    </row>
-    <row r="30" spans="1:12" ht="14.25" customHeight="1">
-      <c r="C30" s="30"/>
-    </row>
-    <row r="31" spans="1:12" ht="14.25" customHeight="1"/>
-    <row r="32" spans="1:12" ht="14.25" customHeight="1"/>
-    <row r="33" ht="14.25" customHeight="1"/>
-    <row r="34" ht="14.25" customHeight="1"/>
-    <row r="35" ht="14.25" customHeight="1"/>
-    <row r="36" ht="14.25" customHeight="1"/>
-    <row r="37" ht="14.25" customHeight="1"/>
-    <row r="38" ht="14.25" customHeight="1"/>
-    <row r="39" ht="14.25" customHeight="1"/>
-    <row r="40" ht="14.25" customHeight="1"/>
-    <row r="41" ht="14.25" customHeight="1"/>
-    <row r="42" ht="14.25" customHeight="1"/>
-    <row r="43" ht="14.25" customHeight="1"/>
-    <row r="44" ht="14.25" customHeight="1"/>
-    <row r="45" ht="14.25" customHeight="1"/>
-    <row r="46" ht="14.25" customHeight="1"/>
-    <row r="47" ht="14.25" customHeight="1"/>
-    <row r="48" ht="14.25" customHeight="1"/>
+      <c r="C25" s="41"/>
+    </row>
+    <row r="26" spans="1:12" ht="14.25" customHeight="1"/>
+    <row r="27" spans="1:12" ht="14.25" customHeight="1"/>
+    <row r="28" spans="1:12" ht="14.25" customHeight="1"/>
+    <row r="29" spans="1:12" ht="14.25" customHeight="1"/>
+    <row r="30" spans="1:12" ht="14.25" customHeight="1"/>
+    <row r="31" spans="1:12" ht="14.25" customHeight="1">
+      <c r="A31" s="18"/>
+      <c r="E31" s="18"/>
+      <c r="I31" s="18"/>
+      <c r="J31" s="18"/>
+      <c r="K31" s="18"/>
+    </row>
+    <row r="32" spans="1:12" ht="14.25" customHeight="1">
+      <c r="A32" s="18"/>
+      <c r="B32" s="18"/>
+      <c r="C32" s="22"/>
+      <c r="D32" s="18"/>
+      <c r="E32" s="18"/>
+      <c r="F32" s="18"/>
+      <c r="G32" s="18"/>
+      <c r="H32" s="18"/>
+      <c r="I32" s="18"/>
+      <c r="J32" s="18"/>
+      <c r="K32" s="18"/>
+    </row>
+    <row r="33" spans="3:3" ht="14.25" customHeight="1">
+      <c r="C33" s="22"/>
+    </row>
+    <row r="34" spans="3:3" ht="14.25" customHeight="1">
+      <c r="C34" s="22"/>
+    </row>
+    <row r="35" spans="3:3" ht="14.25" customHeight="1">
+      <c r="C35" s="22"/>
+    </row>
+    <row r="36" spans="3:3" ht="14.25" customHeight="1">
+      <c r="C36" s="22"/>
+    </row>
+    <row r="37" spans="3:3" ht="14.25" customHeight="1"/>
+    <row r="38" spans="3:3" ht="14.25" customHeight="1"/>
+    <row r="39" spans="3:3" ht="14.25" customHeight="1"/>
+    <row r="40" spans="3:3" ht="14.25" customHeight="1"/>
+    <row r="41" spans="3:3" ht="14.25" customHeight="1"/>
+    <row r="42" spans="3:3" ht="14.25" customHeight="1"/>
+    <row r="43" spans="3:3" ht="14.25" customHeight="1"/>
+    <row r="44" spans="3:3" ht="14.25" customHeight="1"/>
+    <row r="45" spans="3:3" ht="14.25" customHeight="1"/>
+    <row r="46" spans="3:3" ht="14.25" customHeight="1"/>
+    <row r="47" spans="3:3" ht="14.25" customHeight="1"/>
+    <row r="48" spans="3:3" ht="14.25" customHeight="1"/>
     <row r="49" ht="14.25" customHeight="1"/>
     <row r="50" ht="14.25" customHeight="1"/>
     <row r="51" ht="14.25" customHeight="1"/>
@@ -1163,12 +1438,12 @@
     <row r="97" ht="14.25" customHeight="1"/>
     <row r="98" ht="14.25" customHeight="1"/>
     <row r="99" ht="14.25" customHeight="1"/>
-    <row r="100" ht="15.75" customHeight="1"/>
-    <row r="101" ht="15.75" customHeight="1"/>
-    <row r="102" ht="15.75" customHeight="1"/>
-    <row r="103" ht="15.75" customHeight="1"/>
-    <row r="104" ht="15.75" customHeight="1"/>
-    <row r="105" ht="15.75" customHeight="1"/>
+    <row r="100" ht="14.25" customHeight="1"/>
+    <row r="101" ht="14.25" customHeight="1"/>
+    <row r="102" ht="14.25" customHeight="1"/>
+    <row r="103" ht="14.25" customHeight="1"/>
+    <row r="104" ht="14.25" customHeight="1"/>
+    <row r="105" ht="14.25" customHeight="1"/>
     <row r="106" ht="15.75" customHeight="1"/>
     <row r="107" ht="15.75" customHeight="1"/>
     <row r="108" ht="15.75" customHeight="1"/>
@@ -2063,20 +2338,28 @@
     <row r="997" ht="15.75" customHeight="1"/>
     <row r="998" ht="15.75" customHeight="1"/>
     <row r="999" ht="15.75" customHeight="1"/>
+    <row r="1000" ht="15.75" customHeight="1"/>
+    <row r="1001" ht="15.75" customHeight="1"/>
+    <row r="1002" ht="15.75" customHeight="1"/>
+    <row r="1003" ht="15.75" customHeight="1"/>
+    <row r="1004" ht="15.75" customHeight="1"/>
+    <row r="1005" ht="15.75" customHeight="1"/>
   </sheetData>
-  <mergeCells count="12">
-    <mergeCell ref="D9:D12"/>
-    <mergeCell ref="E7:E8"/>
-    <mergeCell ref="E9:E12"/>
-    <mergeCell ref="A2:A3"/>
-    <mergeCell ref="C7:C8"/>
-    <mergeCell ref="D7:D8"/>
-    <mergeCell ref="B2:B3"/>
-    <mergeCell ref="A4:A8"/>
-    <mergeCell ref="B4:B8"/>
-    <mergeCell ref="A9:A12"/>
-    <mergeCell ref="B9:B12"/>
-    <mergeCell ref="C9:C12"/>
+  <mergeCells count="14">
+    <mergeCell ref="A17:A18"/>
+    <mergeCell ref="B17:B18"/>
+    <mergeCell ref="C11:C12"/>
+    <mergeCell ref="C13:C14"/>
+    <mergeCell ref="C15:C16"/>
+    <mergeCell ref="B10:B16"/>
+    <mergeCell ref="A2:A9"/>
+    <mergeCell ref="B2:B9"/>
+    <mergeCell ref="C3:C4"/>
+    <mergeCell ref="C6:C7"/>
+    <mergeCell ref="C8:C9"/>
+    <mergeCell ref="A10:A16"/>
+    <mergeCell ref="D17:D18"/>
+    <mergeCell ref="D14:D15"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Updated RTM with new SRS specifications Signed-off-by: moamen-ahmed-93 <moamen.ahmed.9930@gmail.com>
</commit_message>
<xml_diff>
--- a/Software specification/RTM.xlsx
+++ b/Software specification/RTM.xlsx
@@ -1,34 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22430"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Moamen\Desktop\SWE\Software specification\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3EE5007-6290-4CE4-BE54-214D83FE89BA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
-  <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
-  </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet state="visible" name="Sheet1" sheetId="1" r:id="rId4"/>
   </sheets>
   <definedNames>
-    <definedName name="_Toc30697436" localSheetId="0">Sheet1!$I$11</definedName>
+    <definedName localSheetId="0" name="_Toc30697436">Sheet1!$F$11</definedName>
   </definedNames>
-  <calcPr calcId="0"/>
-  <extLst>
-    <ext uri="GoogleSheetsCustomDataVersion1">
-      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId5" roundtripDataSignature="AMtx7mjUUwAN8L3rIpndgcaxzZP+i5AGww=="/>
-    </ext>
-  </extLst>
+  <calcPr/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="50">
   <si>
     <t>Requirment ID</t>
   </si>
@@ -39,198 +24,176 @@
     <t>CYRS Requirment ID</t>
   </si>
   <si>
+    <t>SRS Requirment ID</t>
+  </si>
+  <si>
     <t>Version</t>
   </si>
   <si>
-    <t>CYRS Status</t>
-  </si>
-  <si>
-    <t>SRS Requirment ID</t>
-  </si>
-  <si>
-    <t>SRS Status</t>
-  </si>
-  <si>
     <t>HSI Requirment ID</t>
   </si>
   <si>
-    <t>HSI Status</t>
-  </si>
-  <si>
     <t>Req_ PO1_DGC_CRS_01_V1.0</t>
-  </si>
-  <si>
-    <t>v1.0</t>
-  </si>
-  <si>
-    <t>Req_PO1_DGC_SRS_001_v1.0</t>
-  </si>
-  <si>
-    <t>Req_ PO1_DGC_CRS_02_V1.0</t>
-  </si>
-  <si>
-    <t>Req_PO1_DGC_CYRS_003_v1.0</t>
-  </si>
-  <si>
-    <t>Req_PO1_DGC_SRS_002_v1.0</t>
-  </si>
-  <si>
-    <t>Req_PO1_DGC_SRS_003_v1.0</t>
-  </si>
-  <si>
-    <t>Req_PO1_DGC_SRS_004_v1.0</t>
-  </si>
-  <si>
-    <t>Req_PO1_DGC_SRS_005_v1.0</t>
-  </si>
-  <si>
-    <t>Req_ PO1_DGC_CRS_03_V1.0</t>
-  </si>
-  <si>
-    <t>v1.1</t>
-  </si>
-  <si>
-    <t>Req_PO1_DGC_SRS_006_v1.0</t>
-  </si>
-  <si>
-    <t>Req_PO1_DGC_SRS_007_v1.0</t>
-  </si>
-  <si>
-    <t>Req_PO1_DGC_SRS_008_v1.0</t>
-  </si>
-  <si>
-    <t>When the user press any key , it must be followed by a tune</t>
-  </si>
-  <si>
-    <t>Req_PO1_DGC_SRS_010_v1.0</t>
   </si>
   <si>
     <t>The digital calculator should have buttons for all basic mathematical
 operations and button to open/close calculator.</t>
   </si>
   <si>
+    <t>Req_PO1_DGC_CYRS_001_v1.1</t>
+  </si>
+  <si>
     <t xml:space="preserve">HWC_DGC_HSI_001_v1.1 </t>
   </si>
   <si>
-    <t>Proposed</t>
-  </si>
-  <si>
-    <t xml:space="preserve">HWC_DGC_HSI_002_v1.1 </t>
-  </si>
-  <si>
-    <t>HWC_DGC_HSI_004_v1.1</t>
-  </si>
-  <si>
-    <t>HWC_DGC_HSI_003_v1.1</t>
-  </si>
-  <si>
-    <t>Req_PO1_DGC_CYRS_001_v1.1</t>
-  </si>
-  <si>
     <t xml:space="preserve">Req_PO1_DGC_CYRS_002_v1.2 </t>
   </si>
   <si>
+    <t>Req_PO1_DGC_SRS_001_v1.0</t>
+  </si>
+  <si>
+    <t>v1.0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Req_PO1_DGC_CYRS_009_v1.0 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Req_PO1_DGC_SRS_018_v1.1
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Req_PO1_DGC_CYRS_010_v1.0 </t>
+  </si>
+  <si>
+    <t>Req_PO1_DGC_SRS_019_v1.1</t>
+  </si>
+  <si>
+    <t>Req_PO1_DGC_SRS_020_v1.1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Req_PO1_DGC_CYRS_011_v1.0 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Req_PO1_DGC_SRS_021_v1.1
+</t>
+  </si>
+  <si>
+    <t>Req_PO1_DGC_SRS_022_v1.1</t>
+  </si>
+  <si>
+    <t>Req_ PO1_DGC_CRS_02_V1.0</t>
+  </si>
+  <si>
+    <t>The user should enter the numbers and select the operation</t>
+  </si>
+  <si>
+    <t>Req_PO1_DGC_CYRS_003_v1.0</t>
+  </si>
+  <si>
+    <t>Req_PO1_DGC_SRS_002_v1.1</t>
+  </si>
+  <si>
+    <t>Req_PO1_DGC_SRS_003_v1.1</t>
+  </si>
+  <si>
     <t>Req_PO1_DGC_CYRS_004_v1.1</t>
   </si>
   <si>
+    <t>Req_PO1_DGC_SRS_004_v1.1</t>
+  </si>
+  <si>
+    <t>Req_PO1_DGC_SRS_005_v1.1</t>
+  </si>
+  <si>
+    <t>Req_PO1_DGC_SRS_006_v1.1</t>
+  </si>
+  <si>
+    <t>Req_PO1_DGC_SRS_007_v1.1</t>
+  </si>
+  <si>
+    <t>Req_PO1_DGC_SRS_008_v1.1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Req_PO1_DGC_SRS_009_v1.1
+</t>
+  </si>
+  <si>
     <t xml:space="preserve">Req_PO1_DGC_CYRS_005_v1.0 </t>
   </si>
   <si>
+    <t>Req_PO1_DGC_SRS_010_v1.1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Req_PO1_DGC_CYRS_008_v1.0 </t>
+  </si>
+  <si>
+    <t>Req_PO1_DGC_SRS_016_v1.1</t>
+  </si>
+  <si>
+    <t>Req_PO1_DGC_SRS_017_v1.1</t>
+  </si>
+  <si>
+    <t>Req_ PO1_DGC_CRS_03_V1.0</t>
+  </si>
+  <si>
+    <t>Pressing the equal button displays both the operations and result.</t>
+  </si>
+  <si>
     <t xml:space="preserve">Req_PO1_DGC_CYRS_006_v1.1 </t>
   </si>
   <si>
+    <t>Req_PO1_DGC_SRS_011_v1.1</t>
+  </si>
+  <si>
+    <t>Req_PO1_DGC_SRS_012_v1.1</t>
+  </si>
+  <si>
+    <t>Req_PO1_DGC_SRS_013_v1.1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Req_PO1_DGC_CYRS_012_v1.0 </t>
+  </si>
+  <si>
+    <t>Req_PO1_DGC_SRS_023_v1.1</t>
+  </si>
+  <si>
+    <t>When the user press any key , it must be followed by a tune</t>
+  </si>
+  <si>
     <t xml:space="preserve">Req_PO1_DGC_CYRS_007_v1.1 </t>
   </si>
   <si>
-    <t>v1.2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Req_PO1_DGC_CYRS_008_v1.0 </t>
-  </si>
-  <si>
-    <t>The user should enter the numbers and select the operation</t>
-  </si>
-  <si>
-    <t>Pressing the equal button displays both the operations and result.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Req_PO1_DGC_CYRS_009_v1.0 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Req_PO1_DGC_CYRS_010_v1.0 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Req_PO1_DGC_CYRS_011_v1.0 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Req_PO1_DGC_CYRS_012_v1.0 </t>
-  </si>
-  <si>
-    <t>Req_PO1_DGC_SRS_0010_v1.0</t>
-  </si>
-  <si>
-    <t>Req_PO1_DGC_SRS_0011_v1.0</t>
-  </si>
-  <si>
-    <t>Req_PO1_DGC_SRS_0012_v1.0</t>
-  </si>
-  <si>
-    <t>Req_PO1_DGC_SRS_0013_v1.0</t>
-  </si>
-  <si>
-    <t>Req_PO1_DGC_SRS_0014_v1.0</t>
-  </si>
-  <si>
-    <t>Req_PO1_DGC_SRS_0015_v1.0</t>
-  </si>
-  <si>
-    <t>Req_PO1_DGC_SRS_0016_v1.0</t>
-  </si>
-  <si>
-    <t>Req_PO1_DGC_SRS_0017_v1.0</t>
+    <t>Req_PO1_DGC_SRS_014_v1.1</t>
+  </si>
+  <si>
+    <t>Req_PO1_DGC_SRS_015_v1.1</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <fonts count="5">
     <font>
-      <sz val="11"/>
+      <sz val="11.0"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
     </font>
     <font>
       <b/>
-      <sz val="12"/>
+      <sz val="12.0"/>
       <color rgb="FF757070"/>
       <name val="Calibri"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
+      <sz val="11.0"/>
+      <color theme="1"/>
       <name val="Calibri"/>
     </font>
+    <font/>
     <font>
-      <sz val="11"/>
+      <sz val="11.0"/>
       <name val="Calibri"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="3">
@@ -238,7 +201,7 @@
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="gray125"/>
+      <patternFill patternType="lightGray"/>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -247,14 +210,8 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="14">
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
+  <borders count="10">
+    <border/>
     <border>
       <left style="thin">
         <color rgb="FF000000"/>
@@ -262,11 +219,9 @@
       <right style="thin">
         <color rgb="FF000000"/>
       </right>
-      <top/>
       <bottom style="thin">
         <color rgb="FF000000"/>
       </bottom>
-      <diagonal/>
     </border>
     <border>
       <left style="thin">
@@ -278,19 +233,14 @@
       <top style="thin">
         <color rgb="FF000000"/>
       </top>
-      <bottom/>
-      <diagonal/>
     </border>
     <border>
       <left style="thin">
         <color rgb="FF000000"/>
       </left>
-      <right/>
       <top style="thin">
         <color rgb="FF000000"/>
       </top>
-      <bottom/>
-      <diagonal/>
     </border>
     <border>
       <left style="thin">
@@ -299,18 +249,24 @@
       <right style="thin">
         <color rgb="FF000000"/>
       </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
     </border>
     <border>
-      <left/>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+    </border>
+    <border>
       <right style="thin">
         <color rgb="FF000000"/>
       </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
     </border>
     <border>
       <left style="thin">
@@ -325,306 +281,138 @@
       <bottom style="thin">
         <color rgb="FF000000"/>
       </bottom>
-      <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF000000"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF000000"/>
-      </left>
-      <right/>
-      <top/>
       <bottom style="thin">
         <color rgb="FF000000"/>
       </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF000000"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="67">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+  <cellXfs count="39">
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    </xf>
+    <xf borderId="1" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf borderId="2" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf borderId="3" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
+    </xf>
+    <xf borderId="2" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
+    </xf>
+    <xf borderId="2" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf borderId="2" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf borderId="4" fillId="0" fontId="3" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="5" fillId="0" fontId="3" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="4" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
+    </xf>
+    <xf borderId="1" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf borderId="4" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf borderId="4" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf borderId="4" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
+    </xf>
+    <xf borderId="5" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf borderId="4" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf borderId="1" fillId="0" fontId="3" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="6" fillId="0" fontId="3" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="2" fillId="2" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0" vertical="center"/>
+    </xf>
+    <xf borderId="3" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf borderId="2" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0" vertical="center"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf borderId="4" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf borderId="4" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0" vertical="center"/>
+    </xf>
+    <xf borderId="7" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf borderId="4" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf borderId="4" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf borderId="1" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0" vertical="center"/>
+    </xf>
+    <xf borderId="1" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf borderId="2" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf borderId="2" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0" vertical="center"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf borderId="8" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf borderId="8" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf borderId="9" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0" vertical="center"/>
+    </xf>
+    <xf borderId="1" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle xfId="0" name="Normal" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Sheets">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheets">
   <a:themeElements>
     <a:clrScheme name="Sheets">
       <a:dk1>
@@ -814,36 +602,30 @@
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
-  <a:objectDefaults/>
-  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L1005"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+  <sheetPr>
+    <pageSetUpPr/>
+  </sheetPr>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F29" sqref="F29"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.0"/>
   <cols>
-    <col min="1" max="1" width="29.140625" customWidth="1"/>
-    <col min="2" max="2" width="61.7109375" customWidth="1"/>
-    <col min="3" max="3" width="43" customWidth="1"/>
-    <col min="4" max="4" width="8.7109375" hidden="1" customWidth="1"/>
-    <col min="5" max="5" width="13.42578125" customWidth="1"/>
-    <col min="6" max="6" width="29.5703125" customWidth="1"/>
-    <col min="7" max="7" width="8.7109375" hidden="1" customWidth="1"/>
-    <col min="8" max="8" width="11.140625" customWidth="1"/>
-    <col min="9" max="9" width="23.42578125" customWidth="1"/>
-    <col min="10" max="10" width="8.7109375" hidden="1" customWidth="1"/>
-    <col min="11" max="11" width="10.5703125" customWidth="1"/>
-    <col min="12" max="12" width="8.7109375" customWidth="1"/>
+    <col customWidth="1" min="1" max="1" width="29.14"/>
+    <col customWidth="1" min="2" max="2" width="61.71"/>
+    <col customWidth="1" min="3" max="3" width="43.0"/>
+    <col customWidth="1" min="4" max="4" width="29.57"/>
+    <col customWidth="1" hidden="1" min="5" max="5" width="8.71"/>
+    <col customWidth="1" min="6" max="6" width="23.43"/>
+    <col customWidth="1" hidden="1" min="7" max="7" width="8.71"/>
+    <col customWidth="1" min="8" max="8" width="8.71"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="14.25" customHeight="1">
+    <row r="1" ht="14.25" customHeight="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -863,530 +645,425 @@
         <v>5</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="H1" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" ht="14.25" customHeight="1">
+      <c r="A2" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="B2" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="J1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="K1" s="1" t="s">
+      <c r="C2" s="4" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="2" spans="1:12" ht="14.25" customHeight="1">
-      <c r="A2" s="27" t="s">
+      <c r="D2" s="5"/>
+      <c r="E2" s="6"/>
+      <c r="F2" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="B2" s="48" t="s">
+      <c r="G2" s="6"/>
+      <c r="H2" s="7"/>
+    </row>
+    <row r="3" ht="14.25" customHeight="1">
+      <c r="A3" s="8"/>
+      <c r="B3" s="9"/>
+      <c r="C3" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="D3" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="E3" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="F3" s="12"/>
+      <c r="G3" s="11"/>
+      <c r="H3" s="7"/>
+    </row>
+    <row r="4" ht="14.25" customHeight="1">
+      <c r="A4" s="8"/>
+      <c r="B4" s="9"/>
+      <c r="C4" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="D4" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="E4" s="15"/>
+      <c r="F4" s="16"/>
+      <c r="G4" s="15"/>
+      <c r="H4" s="7"/>
+    </row>
+    <row r="5" ht="14.25" customHeight="1">
+      <c r="A5" s="8"/>
+      <c r="B5" s="9"/>
+      <c r="C5" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="D5" s="14" t="s">
+        <v>16</v>
+      </c>
+      <c r="E5" s="15"/>
+      <c r="F5" s="16"/>
+      <c r="G5" s="15"/>
+      <c r="H5" s="7"/>
+    </row>
+    <row r="6" ht="14.25" customHeight="1">
+      <c r="A6" s="8"/>
+      <c r="B6" s="9"/>
+      <c r="C6" s="8"/>
+      <c r="D6" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="E6" s="15"/>
+      <c r="F6" s="16"/>
+      <c r="G6" s="15"/>
+      <c r="H6" s="7"/>
+    </row>
+    <row r="7" ht="14.25" customHeight="1">
+      <c r="A7" s="8"/>
+      <c r="B7" s="9"/>
+      <c r="C7" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="D7" s="14" t="s">
+        <v>19</v>
+      </c>
+      <c r="E7" s="15"/>
+      <c r="F7" s="16"/>
+      <c r="G7" s="15"/>
+      <c r="H7" s="7"/>
+    </row>
+    <row r="8" ht="14.25" customHeight="1">
+      <c r="A8" s="17"/>
+      <c r="B8" s="18"/>
+      <c r="C8" s="17"/>
+      <c r="D8" s="14" t="s">
+        <v>20</v>
+      </c>
+      <c r="E8" s="15"/>
+      <c r="F8" s="16"/>
+      <c r="G8" s="15"/>
+      <c r="H8" s="7"/>
+    </row>
+    <row r="9" ht="15.0" customHeight="1">
+      <c r="A9" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C9" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="D9" s="19" t="s">
+        <v>24</v>
+      </c>
+      <c r="E9" s="20" t="s">
+        <v>12</v>
+      </c>
+      <c r="F9" s="21"/>
+      <c r="G9" s="6"/>
+      <c r="H9" s="7"/>
+    </row>
+    <row r="10" ht="14.25" customHeight="1">
+      <c r="A10" s="8"/>
+      <c r="B10" s="8"/>
+      <c r="C10" s="8"/>
+      <c r="D10" s="22" t="s">
         <v>25</v>
       </c>
-      <c r="C2" s="49" t="s">
+      <c r="E10" s="23"/>
+      <c r="F10" s="24"/>
+      <c r="G10" s="24"/>
+      <c r="H10" s="7"/>
+    </row>
+    <row r="11" ht="14.25" customHeight="1">
+      <c r="A11" s="8"/>
+      <c r="B11" s="8"/>
+      <c r="C11" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="D11" s="25" t="s">
+        <v>27</v>
+      </c>
+      <c r="E11" s="24" t="s">
+        <v>12</v>
+      </c>
+      <c r="F11" s="24"/>
+      <c r="G11" s="24"/>
+      <c r="H11" s="7"/>
+    </row>
+    <row r="12" ht="14.25" customHeight="1">
+      <c r="A12" s="8"/>
+      <c r="B12" s="8"/>
+      <c r="C12" s="8"/>
+      <c r="D12" s="25" t="s">
+        <v>28</v>
+      </c>
+      <c r="E12" s="24"/>
+      <c r="F12" s="26"/>
+      <c r="G12" s="24"/>
+      <c r="H12" s="7"/>
+    </row>
+    <row r="13" ht="14.25" customHeight="1">
+      <c r="A13" s="8"/>
+      <c r="B13" s="8"/>
+      <c r="C13" s="8"/>
+      <c r="D13" s="25" t="s">
+        <v>29</v>
+      </c>
+      <c r="E13" s="24"/>
+      <c r="F13" s="26"/>
+      <c r="G13" s="24"/>
+      <c r="H13" s="7"/>
+    </row>
+    <row r="14" ht="14.25" customHeight="1">
+      <c r="A14" s="8"/>
+      <c r="B14" s="8"/>
+      <c r="C14" s="8"/>
+      <c r="D14" s="25" t="s">
+        <v>30</v>
+      </c>
+      <c r="E14" s="24"/>
+      <c r="F14" s="26"/>
+      <c r="G14" s="24"/>
+      <c r="H14" s="7"/>
+    </row>
+    <row r="15" ht="14.25" customHeight="1">
+      <c r="A15" s="8"/>
+      <c r="B15" s="8"/>
+      <c r="C15" s="8"/>
+      <c r="D15" s="25" t="s">
         <v>31</v>
       </c>
-      <c r="D2" s="24" t="s">
-        <v>19</v>
-      </c>
-      <c r="E2" s="24"/>
-      <c r="F2" s="3"/>
-      <c r="G2" s="4"/>
-      <c r="H2" s="4"/>
-      <c r="I2" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="J2" s="4"/>
-      <c r="K2" s="24" t="s">
-        <v>27</v>
-      </c>
-      <c r="L2" s="6"/>
-    </row>
-    <row r="3" spans="1:12" ht="14.25" customHeight="1">
-      <c r="A3" s="30"/>
-      <c r="B3" s="45"/>
-      <c r="C3" s="50" t="s">
+      <c r="E15" s="24"/>
+      <c r="F15" s="26"/>
+      <c r="G15" s="24"/>
+      <c r="H15" s="7"/>
+    </row>
+    <row r="16" ht="14.25" customHeight="1">
+      <c r="A16" s="8"/>
+      <c r="B16" s="8"/>
+      <c r="C16" s="8"/>
+      <c r="D16" s="25" t="s">
         <v>32</v>
       </c>
-      <c r="D3" s="32" t="s">
+      <c r="E16" s="24"/>
+      <c r="F16" s="26"/>
+      <c r="G16" s="24"/>
+      <c r="H16" s="7"/>
+    </row>
+    <row r="17" ht="14.25" customHeight="1">
+      <c r="A17" s="8"/>
+      <c r="B17" s="8"/>
+      <c r="C17" s="27" t="s">
+        <v>33</v>
+      </c>
+      <c r="D17" s="25" t="s">
+        <v>34</v>
+      </c>
+      <c r="E17" s="24" t="s">
+        <v>12</v>
+      </c>
+      <c r="F17" s="26"/>
+      <c r="G17" s="24"/>
+      <c r="H17" s="7"/>
+    </row>
+    <row r="18" ht="15.0" customHeight="1">
+      <c r="A18" s="8"/>
+      <c r="B18" s="8"/>
+      <c r="C18" s="28" t="s">
+        <v>35</v>
+      </c>
+      <c r="D18" s="25" t="s">
+        <v>36</v>
+      </c>
+      <c r="E18" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="F18" s="16"/>
+      <c r="G18" s="11"/>
+      <c r="H18" s="7"/>
+    </row>
+    <row r="19" ht="15.0" customHeight="1">
+      <c r="A19" s="17"/>
+      <c r="B19" s="17"/>
+      <c r="C19" s="17"/>
+      <c r="D19" s="29" t="s">
         <v>37</v>
       </c>
-      <c r="E3" s="12"/>
-      <c r="F3" s="56" t="s">
-        <v>11</v>
-      </c>
-      <c r="G3" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="H3" s="37" t="s">
-        <v>27</v>
-      </c>
-      <c r="I3" s="31" t="s">
-        <v>28</v>
-      </c>
-      <c r="J3" s="9"/>
-      <c r="K3" s="37" t="s">
-        <v>27</v>
-      </c>
-      <c r="L3" s="6"/>
-    </row>
-    <row r="4" spans="1:12" ht="14.25" customHeight="1">
-      <c r="A4" s="30"/>
-      <c r="B4" s="45"/>
-      <c r="C4" s="50"/>
-      <c r="D4" s="43"/>
-      <c r="E4" s="12"/>
-      <c r="F4" s="56" t="s">
-        <v>14</v>
-      </c>
-      <c r="G4" s="38"/>
-      <c r="H4" s="37" t="s">
-        <v>27</v>
-      </c>
-      <c r="I4" s="31"/>
-      <c r="J4" s="12"/>
-      <c r="K4" s="37"/>
-      <c r="L4" s="6"/>
-    </row>
-    <row r="5" spans="1:12" ht="14.25" customHeight="1">
-      <c r="A5" s="30"/>
-      <c r="B5" s="45"/>
-      <c r="C5" s="44" t="s">
+      <c r="E19" s="24"/>
+      <c r="F19" s="30"/>
+      <c r="G19" s="24"/>
+      <c r="H19" s="7"/>
+    </row>
+    <row r="20" ht="14.25" customHeight="1">
+      <c r="A20" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="C20" s="31" t="s">
+        <v>40</v>
+      </c>
+      <c r="D20" s="32" t="s">
         <v>41</v>
       </c>
-      <c r="D5" s="43"/>
-      <c r="E5" s="12"/>
-      <c r="F5" s="56" t="s">
+      <c r="E20" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="F20" s="21"/>
+      <c r="G20" s="6"/>
+      <c r="H20" s="7"/>
+    </row>
+    <row r="21" ht="14.25" customHeight="1">
+      <c r="A21" s="8"/>
+      <c r="B21" s="8"/>
+      <c r="C21" s="8"/>
+      <c r="D21" s="25" t="s">
+        <v>42</v>
+      </c>
+      <c r="E21" s="24"/>
+      <c r="F21" s="16"/>
+      <c r="G21" s="24"/>
+      <c r="H21" s="7"/>
+    </row>
+    <row r="22" ht="14.25" customHeight="1">
+      <c r="A22" s="8"/>
+      <c r="B22" s="8"/>
+      <c r="C22" s="8"/>
+      <c r="D22" s="25" t="s">
+        <v>43</v>
+      </c>
+      <c r="E22" s="24"/>
+      <c r="F22" s="16"/>
+      <c r="G22" s="24"/>
+      <c r="H22" s="7"/>
+    </row>
+    <row r="23" ht="14.25" customHeight="1">
+      <c r="A23" s="8"/>
+      <c r="B23" s="8"/>
+      <c r="C23" s="33" t="s">
+        <v>44</v>
+      </c>
+      <c r="D23" s="25" t="s">
+        <v>45</v>
+      </c>
+      <c r="E23" s="24" t="s">
+        <v>12</v>
+      </c>
+      <c r="F23" s="16"/>
+      <c r="G23" s="24"/>
+      <c r="H23" s="7"/>
+    </row>
+    <row r="24" ht="14.25" customHeight="1">
+      <c r="A24" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="B24" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="C24" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="G5" s="38"/>
-      <c r="H5" s="37" t="s">
-        <v>27</v>
-      </c>
-      <c r="I5" s="31"/>
-      <c r="J5" s="38"/>
-      <c r="K5" s="65"/>
-      <c r="L5" s="6"/>
-    </row>
-    <row r="6" spans="1:12" ht="14.25" customHeight="1">
-      <c r="A6" s="30"/>
-      <c r="B6" s="45"/>
-      <c r="C6" s="51" t="s">
-        <v>42</v>
-      </c>
-      <c r="D6" s="43"/>
-      <c r="E6" s="12"/>
-      <c r="F6" s="56" t="s">
+      <c r="D24" s="32" t="s">
         <v>48</v>
       </c>
-      <c r="G6" s="38"/>
-      <c r="H6" s="37" t="s">
-        <v>27</v>
-      </c>
-      <c r="I6" s="31"/>
-      <c r="J6" s="38"/>
-      <c r="K6" s="65"/>
-      <c r="L6" s="6"/>
-    </row>
-    <row r="7" spans="1:12" ht="14.25" customHeight="1">
-      <c r="A7" s="30"/>
-      <c r="B7" s="45"/>
-      <c r="C7" s="51"/>
-      <c r="D7" s="43"/>
-      <c r="E7" s="12"/>
-      <c r="F7" s="56" t="s">
+      <c r="E24" s="34" t="s">
+        <v>12</v>
+      </c>
+      <c r="F24" s="21"/>
+      <c r="G24" s="35"/>
+      <c r="H24" s="7"/>
+    </row>
+    <row r="25" ht="14.25" customHeight="1">
+      <c r="A25" s="17"/>
+      <c r="B25" s="17"/>
+      <c r="C25" s="17"/>
+      <c r="D25" s="36" t="s">
         <v>49</v>
       </c>
-      <c r="G7" s="38"/>
-      <c r="H7" s="37" t="s">
-        <v>27</v>
-      </c>
-      <c r="I7" s="31"/>
-      <c r="J7" s="38"/>
-      <c r="K7" s="65"/>
-      <c r="L7" s="6"/>
-    </row>
-    <row r="8" spans="1:12" ht="14.25" customHeight="1">
-      <c r="A8" s="30"/>
-      <c r="B8" s="45"/>
-      <c r="C8" s="51" t="s">
-        <v>43</v>
-      </c>
-      <c r="D8" s="43"/>
-      <c r="E8" s="12"/>
-      <c r="F8" s="56" t="s">
-        <v>50</v>
-      </c>
-      <c r="G8" s="38"/>
-      <c r="H8" s="37" t="s">
-        <v>27</v>
-      </c>
-      <c r="I8" s="31"/>
-      <c r="J8" s="38"/>
-      <c r="K8" s="65"/>
-      <c r="L8" s="6"/>
-    </row>
-    <row r="9" spans="1:12" ht="14.25" customHeight="1">
-      <c r="A9" s="40"/>
-      <c r="B9" s="42"/>
-      <c r="C9" s="52"/>
-      <c r="D9" s="43"/>
-      <c r="E9" s="12"/>
-      <c r="F9" s="56" t="s">
-        <v>51</v>
-      </c>
-      <c r="G9" s="38"/>
-      <c r="H9" s="63" t="s">
-        <v>27</v>
-      </c>
-      <c r="I9" s="31"/>
-      <c r="J9" s="38"/>
-      <c r="K9" s="66"/>
-      <c r="L9" s="6"/>
-    </row>
-    <row r="10" spans="1:12" ht="14.25" customHeight="1">
-      <c r="A10" s="27" t="s">
-        <v>12</v>
-      </c>
-      <c r="B10" s="34" t="s">
-        <v>39</v>
-      </c>
-      <c r="C10" s="53" t="s">
-        <v>13</v>
-      </c>
-      <c r="D10" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="E10" s="2"/>
-      <c r="F10" s="57" t="s">
-        <v>15</v>
-      </c>
-      <c r="G10" s="10" t="s">
-        <v>10</v>
-      </c>
-      <c r="H10" s="37" t="s">
-        <v>27</v>
-      </c>
-      <c r="I10" s="25" t="s">
-        <v>28</v>
-      </c>
-      <c r="J10" s="4"/>
-      <c r="K10" s="37" t="s">
-        <v>27</v>
-      </c>
-      <c r="L10" s="6"/>
-    </row>
-    <row r="11" spans="1:12" ht="14.25" customHeight="1">
-      <c r="A11" s="30"/>
-      <c r="B11" s="33"/>
-      <c r="C11" s="50" t="s">
-        <v>33</v>
-      </c>
-      <c r="D11" s="11" t="s">
-        <v>10</v>
-      </c>
-      <c r="E11" s="11"/>
-      <c r="F11" s="58" t="s">
-        <v>16</v>
-      </c>
-      <c r="G11" s="11" t="s">
-        <v>10</v>
-      </c>
-      <c r="H11" s="37" t="s">
-        <v>27</v>
-      </c>
-      <c r="I11" s="12"/>
-      <c r="J11" s="12"/>
-      <c r="K11" s="12"/>
-      <c r="L11" s="6"/>
-    </row>
-    <row r="12" spans="1:12" ht="14.25" customHeight="1">
-      <c r="A12" s="30"/>
-      <c r="B12" s="33"/>
-      <c r="C12" s="50"/>
-      <c r="D12" s="12"/>
-      <c r="E12" s="12"/>
-      <c r="F12" s="58" t="s">
-        <v>17</v>
-      </c>
-      <c r="G12" s="12"/>
-      <c r="H12" s="37" t="s">
-        <v>27</v>
-      </c>
-      <c r="I12" s="13"/>
-      <c r="J12" s="12"/>
-      <c r="K12" s="12"/>
-      <c r="L12" s="6"/>
-    </row>
-    <row r="13" spans="1:12" ht="14.25" customHeight="1">
-      <c r="A13" s="30"/>
-      <c r="B13" s="33"/>
-      <c r="C13" s="61" t="s">
-        <v>34</v>
-      </c>
-      <c r="D13" s="11" t="s">
-        <v>10</v>
-      </c>
-      <c r="E13" s="12"/>
-      <c r="F13" s="58" t="s">
-        <v>20</v>
-      </c>
-      <c r="G13" s="11" t="s">
-        <v>10</v>
-      </c>
-      <c r="H13" s="37" t="s">
-        <v>27</v>
-      </c>
-      <c r="I13" s="13"/>
-      <c r="J13" s="12"/>
-      <c r="K13" s="12"/>
-      <c r="L13" s="6"/>
-    </row>
-    <row r="14" spans="1:12" ht="15" customHeight="1">
-      <c r="A14" s="30"/>
-      <c r="B14" s="33"/>
-      <c r="C14" s="61"/>
-      <c r="D14" s="30" t="s">
-        <v>10</v>
-      </c>
-      <c r="E14" s="46"/>
-      <c r="F14" s="58" t="s">
-        <v>21</v>
-      </c>
-      <c r="G14" s="11" t="s">
-        <v>10</v>
-      </c>
-      <c r="H14" s="37" t="s">
-        <v>27</v>
-      </c>
-      <c r="I14" s="14"/>
-      <c r="J14" s="12"/>
-      <c r="K14" s="14"/>
-      <c r="L14" s="6"/>
-    </row>
-    <row r="15" spans="1:12" ht="15" customHeight="1">
-      <c r="A15" s="30"/>
-      <c r="B15" s="33"/>
-      <c r="C15" s="33" t="s">
-        <v>38</v>
-      </c>
-      <c r="D15" s="29"/>
-      <c r="E15" s="46"/>
-      <c r="F15" s="58" t="s">
-        <v>45</v>
-      </c>
-      <c r="G15" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="H15" s="37" t="s">
-        <v>27</v>
-      </c>
-      <c r="I15" s="14"/>
-      <c r="J15" s="9"/>
-      <c r="K15" s="14"/>
-      <c r="L15" s="6"/>
-    </row>
-    <row r="16" spans="1:12" ht="15" customHeight="1">
-      <c r="A16" s="40"/>
-      <c r="B16" s="62"/>
-      <c r="C16" s="62"/>
-      <c r="D16" s="23"/>
-      <c r="E16" s="47"/>
-      <c r="F16" s="59" t="s">
-        <v>46</v>
-      </c>
-      <c r="G16" s="12"/>
-      <c r="H16" s="63" t="s">
-        <v>27</v>
-      </c>
-      <c r="I16" s="8"/>
-      <c r="J16" s="12"/>
-      <c r="K16" s="8"/>
-      <c r="L16" s="6"/>
-    </row>
-    <row r="17" spans="1:12" ht="14.25" customHeight="1">
-      <c r="A17" s="27" t="s">
-        <v>18</v>
-      </c>
-      <c r="B17" s="34" t="s">
-        <v>40</v>
-      </c>
-      <c r="C17" s="35" t="s">
-        <v>35</v>
-      </c>
-      <c r="D17" s="27" t="s">
-        <v>19</v>
-      </c>
-      <c r="E17" s="39"/>
-      <c r="F17" s="60" t="s">
-        <v>22</v>
-      </c>
-      <c r="G17" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="H17" s="37" t="s">
-        <v>27</v>
-      </c>
-      <c r="I17" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="J17" s="4"/>
-      <c r="K17" s="24" t="s">
-        <v>27</v>
-      </c>
-      <c r="L17" s="6"/>
-    </row>
-    <row r="18" spans="1:12" ht="14.25" customHeight="1">
-      <c r="A18" s="30"/>
-      <c r="B18" s="33"/>
-      <c r="C18" s="55" t="s">
-        <v>44</v>
-      </c>
-      <c r="D18" s="28"/>
-      <c r="E18" s="36"/>
-      <c r="F18" s="58" t="s">
-        <v>52</v>
-      </c>
-      <c r="G18" s="11" t="s">
-        <v>10</v>
-      </c>
-      <c r="H18" s="37" t="s">
-        <v>27</v>
-      </c>
-      <c r="I18" s="14"/>
-      <c r="J18" s="12"/>
-      <c r="K18" s="14"/>
-      <c r="L18" s="6"/>
-    </row>
-    <row r="19" spans="1:12" ht="14.25" customHeight="1">
-      <c r="A19" s="15" t="s">
-        <v>18</v>
-      </c>
-      <c r="B19" s="15" t="s">
-        <v>23</v>
-      </c>
-      <c r="C19" s="54" t="s">
-        <v>36</v>
-      </c>
-      <c r="D19" s="16" t="s">
-        <v>10</v>
-      </c>
-      <c r="E19" s="17"/>
-      <c r="F19" s="15" t="s">
-        <v>24</v>
-      </c>
-      <c r="G19" s="16" t="s">
-        <v>10</v>
-      </c>
-      <c r="H19" s="64" t="s">
-        <v>27</v>
-      </c>
-      <c r="I19" s="17" t="s">
-        <v>29</v>
-      </c>
-      <c r="J19" s="17"/>
-      <c r="K19" s="26" t="s">
-        <v>27</v>
-      </c>
-      <c r="L19" s="6"/>
-    </row>
-    <row r="20" spans="1:12" ht="14.25" customHeight="1">
-      <c r="L20" s="6"/>
-    </row>
-    <row r="21" spans="1:12" ht="14.25" customHeight="1">
-      <c r="A21" s="18"/>
-      <c r="B21" s="18"/>
-      <c r="C21" s="18"/>
-      <c r="D21" s="18"/>
-      <c r="E21" s="18"/>
-      <c r="F21" s="18"/>
-      <c r="G21" s="18"/>
-      <c r="I21" s="18"/>
-      <c r="J21" s="18"/>
-      <c r="K21" s="18"/>
-      <c r="L21" s="6"/>
-    </row>
-    <row r="22" spans="1:12" ht="14.25" customHeight="1">
-      <c r="A22" s="18"/>
-      <c r="B22" s="18"/>
-      <c r="C22" s="18"/>
-      <c r="D22" s="19"/>
-      <c r="E22" s="20"/>
-      <c r="F22" s="18"/>
-      <c r="G22" s="20"/>
-      <c r="H22" s="21"/>
-      <c r="I22" s="18"/>
-      <c r="J22" s="18"/>
-      <c r="K22" s="18"/>
-      <c r="L22" s="6"/>
-    </row>
-    <row r="23" spans="1:12" ht="14.25" customHeight="1">
-      <c r="C23" s="19"/>
-      <c r="D23" s="19"/>
-      <c r="E23" s="20"/>
-      <c r="F23" s="20"/>
-      <c r="G23" s="20"/>
-      <c r="H23" s="20"/>
-      <c r="I23" s="20"/>
-      <c r="J23" s="20"/>
-      <c r="K23" s="20"/>
-      <c r="L23" s="6"/>
-    </row>
-    <row r="24" spans="1:12" ht="14.25" customHeight="1"/>
-    <row r="25" spans="1:12" ht="14.25" customHeight="1">
-      <c r="C25" s="41"/>
-    </row>
-    <row r="26" spans="1:12" ht="14.25" customHeight="1"/>
-    <row r="27" spans="1:12" ht="14.25" customHeight="1"/>
-    <row r="28" spans="1:12" ht="14.25" customHeight="1"/>
-    <row r="29" spans="1:12" ht="14.25" customHeight="1"/>
-    <row r="30" spans="1:12" ht="14.25" customHeight="1"/>
-    <row r="31" spans="1:12" ht="14.25" customHeight="1">
-      <c r="A31" s="18"/>
-      <c r="E31" s="18"/>
-      <c r="I31" s="18"/>
-      <c r="J31" s="18"/>
-      <c r="K31" s="18"/>
-    </row>
-    <row r="32" spans="1:12" ht="14.25" customHeight="1">
-      <c r="A32" s="18"/>
-      <c r="B32" s="18"/>
-      <c r="C32" s="22"/>
-      <c r="D32" s="18"/>
-      <c r="E32" s="18"/>
-      <c r="F32" s="18"/>
-      <c r="G32" s="18"/>
-      <c r="H32" s="18"/>
-      <c r="I32" s="18"/>
-      <c r="J32" s="18"/>
-      <c r="K32" s="18"/>
-    </row>
-    <row r="33" spans="3:3" ht="14.25" customHeight="1">
-      <c r="C33" s="22"/>
-    </row>
-    <row r="34" spans="3:3" ht="14.25" customHeight="1">
-      <c r="C34" s="22"/>
-    </row>
-    <row r="35" spans="3:3" ht="14.25" customHeight="1">
-      <c r="C35" s="22"/>
-    </row>
-    <row r="36" spans="3:3" ht="14.25" customHeight="1">
-      <c r="C36" s="22"/>
-    </row>
-    <row r="37" spans="3:3" ht="14.25" customHeight="1"/>
-    <row r="38" spans="3:3" ht="14.25" customHeight="1"/>
-    <row r="39" spans="3:3" ht="14.25" customHeight="1"/>
-    <row r="40" spans="3:3" ht="14.25" customHeight="1"/>
-    <row r="41" spans="3:3" ht="14.25" customHeight="1"/>
-    <row r="42" spans="3:3" ht="14.25" customHeight="1"/>
-    <row r="43" spans="3:3" ht="14.25" customHeight="1"/>
-    <row r="44" spans="3:3" ht="14.25" customHeight="1"/>
-    <row r="45" spans="3:3" ht="14.25" customHeight="1"/>
-    <row r="46" spans="3:3" ht="14.25" customHeight="1"/>
-    <row r="47" spans="3:3" ht="14.25" customHeight="1"/>
-    <row r="48" spans="3:3" ht="14.25" customHeight="1"/>
+      <c r="E25" s="23"/>
+      <c r="F25" s="37"/>
+      <c r="G25" s="38"/>
+      <c r="H25" s="7"/>
+    </row>
+    <row r="26" ht="14.25" customHeight="1">
+      <c r="H26" s="7"/>
+    </row>
+    <row r="27" ht="14.25" customHeight="1">
+      <c r="A27" s="38"/>
+      <c r="B27" s="38"/>
+      <c r="C27" s="38"/>
+      <c r="D27" s="38"/>
+      <c r="E27" s="38"/>
+      <c r="F27" s="38"/>
+      <c r="G27" s="38"/>
+      <c r="H27" s="7"/>
+    </row>
+    <row r="28" ht="14.25" customHeight="1">
+      <c r="A28" s="38"/>
+      <c r="B28" s="38"/>
+      <c r="C28" s="38"/>
+      <c r="D28" s="38"/>
+      <c r="E28" s="23"/>
+      <c r="F28" s="38"/>
+      <c r="G28" s="38"/>
+      <c r="H28" s="7"/>
+    </row>
+    <row r="29" ht="14.25" customHeight="1">
+      <c r="C29" s="23"/>
+      <c r="D29" s="23"/>
+      <c r="E29" s="23"/>
+      <c r="F29" s="23"/>
+      <c r="G29" s="23"/>
+      <c r="H29" s="7"/>
+    </row>
+    <row r="30" ht="14.25" customHeight="1"/>
+    <row r="31" ht="14.25" customHeight="1">
+      <c r="C31" s="7"/>
+    </row>
+    <row r="32" ht="14.25" customHeight="1"/>
+    <row r="33" ht="14.25" customHeight="1"/>
+    <row r="34" ht="14.25" customHeight="1"/>
+    <row r="35" ht="14.25" customHeight="1"/>
+    <row r="36" ht="14.25" customHeight="1"/>
+    <row r="37" ht="14.25" customHeight="1">
+      <c r="A37" s="38"/>
+      <c r="F37" s="38"/>
+      <c r="G37" s="38"/>
+    </row>
+    <row r="38" ht="14.25" customHeight="1">
+      <c r="A38" s="38"/>
+      <c r="B38" s="38"/>
+      <c r="C38" s="23"/>
+      <c r="D38" s="38"/>
+      <c r="E38" s="38"/>
+      <c r="F38" s="38"/>
+      <c r="G38" s="38"/>
+    </row>
+    <row r="39" ht="14.25" customHeight="1">
+      <c r="C39" s="23"/>
+    </row>
+    <row r="40" ht="14.25" customHeight="1">
+      <c r="C40" s="23"/>
+    </row>
+    <row r="41" ht="14.25" customHeight="1">
+      <c r="C41" s="23"/>
+    </row>
+    <row r="42" ht="14.25" customHeight="1">
+      <c r="C42" s="23"/>
+    </row>
+    <row r="43" ht="14.25" customHeight="1"/>
+    <row r="44" ht="14.25" customHeight="1"/>
+    <row r="45" ht="14.25" customHeight="1"/>
+    <row r="46" ht="14.25" customHeight="1"/>
+    <row r="47" ht="14.25" customHeight="1"/>
+    <row r="48" ht="14.25" customHeight="1"/>
     <row r="49" ht="14.25" customHeight="1"/>
     <row r="50" ht="14.25" customHeight="1"/>
     <row r="51" ht="14.25" customHeight="1"/>
@@ -1444,12 +1121,12 @@
     <row r="103" ht="14.25" customHeight="1"/>
     <row r="104" ht="14.25" customHeight="1"/>
     <row r="105" ht="14.25" customHeight="1"/>
-    <row r="106" ht="15.75" customHeight="1"/>
-    <row r="107" ht="15.75" customHeight="1"/>
-    <row r="108" ht="15.75" customHeight="1"/>
-    <row r="109" ht="15.75" customHeight="1"/>
-    <row r="110" ht="15.75" customHeight="1"/>
-    <row r="111" ht="15.75" customHeight="1"/>
+    <row r="106" ht="14.25" customHeight="1"/>
+    <row r="107" ht="14.25" customHeight="1"/>
+    <row r="108" ht="14.25" customHeight="1"/>
+    <row r="109" ht="14.25" customHeight="1"/>
+    <row r="110" ht="14.25" customHeight="1"/>
+    <row r="111" ht="14.25" customHeight="1"/>
     <row r="112" ht="15.75" customHeight="1"/>
     <row r="113" ht="15.75" customHeight="1"/>
     <row r="114" ht="15.75" customHeight="1"/>
@@ -2344,24 +2021,28 @@
     <row r="1003" ht="15.75" customHeight="1"/>
     <row r="1004" ht="15.75" customHeight="1"/>
     <row r="1005" ht="15.75" customHeight="1"/>
+    <row r="1006" ht="15.75" customHeight="1"/>
   </sheetData>
-  <mergeCells count="14">
-    <mergeCell ref="A17:A18"/>
-    <mergeCell ref="B17:B18"/>
-    <mergeCell ref="C11:C12"/>
-    <mergeCell ref="C13:C14"/>
-    <mergeCell ref="C15:C16"/>
-    <mergeCell ref="B10:B16"/>
-    <mergeCell ref="A2:A9"/>
-    <mergeCell ref="B2:B9"/>
-    <mergeCell ref="C3:C4"/>
-    <mergeCell ref="C6:C7"/>
-    <mergeCell ref="C8:C9"/>
-    <mergeCell ref="A10:A16"/>
-    <mergeCell ref="D17:D18"/>
-    <mergeCell ref="D14:D15"/>
+  <mergeCells count="15">
+    <mergeCell ref="C7:C8"/>
+    <mergeCell ref="C9:C10"/>
+    <mergeCell ref="C11:C16"/>
+    <mergeCell ref="C18:C19"/>
+    <mergeCell ref="A20:A23"/>
+    <mergeCell ref="A24:A25"/>
+    <mergeCell ref="B24:B25"/>
+    <mergeCell ref="C24:C25"/>
+    <mergeCell ref="C5:C6"/>
+    <mergeCell ref="A9:A19"/>
+    <mergeCell ref="B9:B19"/>
+    <mergeCell ref="B20:B23"/>
+    <mergeCell ref="C20:C22"/>
+    <mergeCell ref="A2:A8"/>
+    <mergeCell ref="B2:B8"/>
   </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <printOptions/>
+  <pageMargins bottom="0.75" footer="0.0" header="0.0" left="0.7" right="0.7" top="0.75"/>
+  <pageSetup orientation="portrait"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>